<commit_message>
gn: update ghana forms
</commit_message>
<xml_diff>
--- a/ONCHO/Breeding Site Survey/Ghana/2022 semptember/gn_oncho_bsa_1_vector_community_question_202210.xlsx
+++ b/ONCHO/Breeding Site Survey/Ghana/2022 semptember/gn_oncho_bsa_1_vector_community_question_202210.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="161">
   <si>
     <t>type</t>
   </si>
@@ -238,6 +238,18 @@
     <t>${c_consent} = 'Yes' and selected(${c_know_oncho}, 'Yes')</t>
   </si>
   <si>
+    <t>geopoint</t>
+  </si>
+  <si>
+    <t>c_gps</t>
+  </si>
+  <si>
+    <t>Enter GPS  </t>
+  </si>
+  <si>
+    <t>Collect GPS coordinates - Must be outside to get accurate reading  </t>
+  </si>
+  <si>
     <t>c_note</t>
   </si>
   <si>
@@ -463,10 +475,10 @@
     <t>allow_choice_duplicates</t>
   </si>
   <si>
-    <t>(2022 October) - 1. vector community questionnaire</t>
-  </si>
-  <si>
-    <t>gn_oncho_bsa_1_vector_community_question_202210</t>
+    <t>(2022 October) - 1. vector community questionnaire V2</t>
+  </si>
+  <si>
+    <t>gn_oncho_bsa_1_vector_community_question_202210_v2</t>
   </si>
   <si>
     <t>English</t>
@@ -495,10 +507,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -541,7 +553,106 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -556,31 +667,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -593,91 +689,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -698,7 +710,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,61 +866,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -776,109 +890,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -935,17 +947,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -980,11 +1006,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1006,26 +1038,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1035,152 +1047,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1232,20 +1244,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1584,14 +1587,14 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomRight" activeCell="C18" sqref="C18:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1646,7 +1649,7 @@
       <c r="L1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="29" t="s">
+      <c r="M1" s="26" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1664,7 +1667,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="19"/>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="24" t="s">
         <v>17</v>
       </c>
       <c r="G2" s="22" t="s">
@@ -1676,8 +1679,8 @@
         <v>19</v>
       </c>
       <c r="K2" s="19"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" s="3" customFormat="1" ht="15.75" spans="1:13">
       <c r="A3" s="18" t="s">
@@ -1693,7 +1696,7 @@
         <v>23</v>
       </c>
       <c r="E3" s="19"/>
-      <c r="F3" s="26"/>
+      <c r="F3" s="24"/>
       <c r="G3" s="22"/>
       <c r="H3" s="19"/>
       <c r="I3" s="19"/>
@@ -1701,8 +1704,8 @@
         <v>19</v>
       </c>
       <c r="K3" s="19"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="18"/>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:13">
       <c r="A4" s="18" t="s">
@@ -1716,7 +1719,7 @@
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="19"/>
-      <c r="F4" s="26"/>
+      <c r="F4" s="24"/>
       <c r="G4" s="22"/>
       <c r="H4" s="19" t="s">
         <v>27</v>
@@ -1726,8 +1729,8 @@
         <v>19</v>
       </c>
       <c r="K4" s="19"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
     </row>
     <row r="5" s="3" customFormat="1" spans="1:13">
       <c r="A5" s="18" t="s">
@@ -1741,7 +1744,7 @@
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="26"/>
+      <c r="F5" s="24"/>
       <c r="G5" s="22"/>
       <c r="H5" s="19" t="s">
         <v>31</v>
@@ -1751,10 +1754,10 @@
         <v>19</v>
       </c>
       <c r="K5" s="19"/>
-      <c r="L5" s="26" t="s">
+      <c r="L5" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="M5" s="23"/>
+      <c r="M5" s="18"/>
     </row>
     <row r="6" s="3" customFormat="1" spans="1:13">
       <c r="A6" s="18" t="s">
@@ -1768,7 +1771,7 @@
       </c>
       <c r="D6" s="20"/>
       <c r="E6" s="19"/>
-      <c r="F6" s="26"/>
+      <c r="F6" s="24"/>
       <c r="G6" s="22"/>
       <c r="H6" s="19" t="s">
         <v>35</v>
@@ -1778,8 +1781,8 @@
         <v>19</v>
       </c>
       <c r="K6" s="19"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="23"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="18"/>
     </row>
     <row r="7" s="3" customFormat="1" ht="30" spans="1:13">
       <c r="A7" s="18" t="s">
@@ -1793,7 +1796,7 @@
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="19"/>
-      <c r="F7" s="26"/>
+      <c r="F7" s="24"/>
       <c r="G7" s="22"/>
       <c r="H7" s="19"/>
       <c r="I7" s="19"/>
@@ -1801,8 +1804,8 @@
         <v>19</v>
       </c>
       <c r="K7" s="19"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
     </row>
     <row r="8" s="3" customFormat="1" ht="15.75" spans="1:13">
       <c r="A8" s="18" t="s">
@@ -1816,7 +1819,7 @@
       </c>
       <c r="D8" s="20"/>
       <c r="E8" s="19"/>
-      <c r="F8" s="26"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="22"/>
       <c r="H8" s="18" t="s">
         <v>42</v>
@@ -1826,8 +1829,8 @@
         <v>19</v>
       </c>
       <c r="K8" s="19"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
     </row>
     <row r="9" s="3" customFormat="1" ht="15.75" spans="1:13">
       <c r="A9" s="18" t="s">
@@ -1840,8 +1843,8 @@
         <v>44</v>
       </c>
       <c r="D9" s="20"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26" t="s">
+      <c r="E9" s="24"/>
+      <c r="F9" s="24" t="s">
         <v>45</v>
       </c>
       <c r="G9" s="20" t="s">
@@ -1855,8 +1858,8 @@
         <v>19</v>
       </c>
       <c r="K9" s="19"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="23"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" s="15" customFormat="1" ht="15.75" customHeight="1" spans="1:13">
       <c r="A10" s="18" t="s">
@@ -1871,7 +1874,7 @@
       <c r="D10" s="20"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="27"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="18" t="s">
         <v>42</v>
       </c>
@@ -1881,7 +1884,7 @@
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="19"/>
-      <c r="M10" s="28"/>
+      <c r="M10" s="24"/>
     </row>
     <row r="11" s="3" customFormat="1" ht="30" spans="1:13">
       <c r="A11" s="18" t="s">
@@ -1898,7 +1901,7 @@
       <c r="F11" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="27" t="s">
+      <c r="G11" s="25" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="18" t="s">
@@ -1910,7 +1913,7 @@
       </c>
       <c r="K11" s="18"/>
       <c r="L11" s="18"/>
-      <c r="M11" s="23"/>
+      <c r="M11" s="18"/>
     </row>
     <row r="12" s="3" customFormat="1" ht="28.5" spans="1:13">
       <c r="A12" s="18" t="s">
@@ -1925,7 +1928,7 @@
       <c r="D12" s="22"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
-      <c r="G12" s="27"/>
+      <c r="G12" s="25"/>
       <c r="H12" s="18" t="s">
         <v>42</v>
       </c>
@@ -1935,7 +1938,7 @@
       </c>
       <c r="K12" s="18"/>
       <c r="L12" s="18"/>
-      <c r="M12" s="23"/>
+      <c r="M12" s="18"/>
     </row>
     <row r="13" s="3" customFormat="1" ht="28.5" spans="1:13">
       <c r="A13" s="18" t="s">
@@ -1952,7 +1955,7 @@
       </c>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="27"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="18" t="s">
         <v>60</v>
       </c>
@@ -1962,7 +1965,7 @@
       </c>
       <c r="K13" s="18"/>
       <c r="L13" s="18"/>
-      <c r="M13" s="23"/>
+      <c r="M13" s="18"/>
     </row>
     <row r="14" s="3" customFormat="1" ht="42.75" spans="1:13">
       <c r="A14" s="18" t="s">
@@ -1979,7 +1982,7 @@
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
-      <c r="G14" s="27"/>
+      <c r="G14" s="25"/>
       <c r="H14" s="18" t="s">
         <v>60</v>
       </c>
@@ -1989,7 +1992,7 @@
       </c>
       <c r="K14" s="18"/>
       <c r="L14" s="18"/>
-      <c r="M14" s="23"/>
+      <c r="M14" s="18"/>
     </row>
     <row r="15" s="3" customFormat="1" ht="15.75" spans="1:13">
       <c r="A15" s="18" t="s">
@@ -2004,7 +2007,7 @@
       <c r="D15" s="22"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18"/>
-      <c r="G15" s="27"/>
+      <c r="G15" s="25"/>
       <c r="H15" s="18" t="s">
         <v>60</v>
       </c>
@@ -2014,7 +2017,7 @@
       </c>
       <c r="K15" s="18"/>
       <c r="L15" s="18"/>
-      <c r="M15" s="23"/>
+      <c r="M15" s="18"/>
     </row>
     <row r="16" s="3" customFormat="1" ht="28.5" spans="1:13">
       <c r="A16" s="18" t="s">
@@ -2029,7 +2032,7 @@
       <c r="D16" s="22"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="27"/>
+      <c r="G16" s="25"/>
       <c r="H16" s="18" t="s">
         <v>42</v>
       </c>
@@ -2039,13 +2042,13 @@
       </c>
       <c r="K16" s="18"/>
       <c r="L16" s="18"/>
-      <c r="M16" s="23"/>
+      <c r="M16" s="18"/>
     </row>
     <row r="17" s="3" customFormat="1" ht="28.5" spans="1:13">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="18" t="s">
         <v>70</v>
       </c>
       <c r="C17" s="22" t="s">
@@ -2054,7 +2057,7 @@
       <c r="D17" s="22"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
-      <c r="G17" s="27"/>
+      <c r="G17" s="25"/>
       <c r="H17" s="21" t="s">
         <v>72</v>
       </c>
@@ -2064,89 +2067,116 @@
       </c>
       <c r="K17" s="18"/>
       <c r="L17" s="18"/>
-      <c r="M17" s="23"/>
-    </row>
-    <row r="18" s="3" customFormat="1" spans="1:13">
-      <c r="A18" s="23" t="s">
+      <c r="M17" s="18"/>
+    </row>
+    <row r="18" s="3" customFormat="1" ht="30" spans="1:13">
+      <c r="A18" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I18" s="18"/>
+      <c r="J18" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="18"/>
+      <c r="L18" s="18"/>
+      <c r="M18" s="18"/>
+    </row>
+    <row r="19" s="3" customFormat="1" spans="1:13">
+      <c r="A19" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="24"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-    </row>
-    <row r="19" s="3" customFormat="1" ht="28.5" spans="1:13">
-      <c r="A19" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19" s="22" t="s">
+      <c r="B19" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="22"/>
+      <c r="C19" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="21"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="18" t="s">
-        <v>78</v>
-      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="18"/>
       <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
+      <c r="J19" s="18"/>
       <c r="K19" s="18"/>
       <c r="L19" s="18"/>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" s="3" customFormat="1" spans="1:13">
+      <c r="M19" s="18"/>
+    </row>
+    <row r="20" s="3" customFormat="1" ht="28.5" spans="1:13">
       <c r="A20" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
+      <c r="C20" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="22"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="25"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-      <c r="K20" s="23"/>
-      <c r="L20" s="23"/>
-      <c r="M20" s="23"/>
+      <c r="H20" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" s="18"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
     </row>
     <row r="21" s="3" customFormat="1" spans="1:13">
       <c r="A21" s="18" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
+        <v>84</v>
+      </c>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+    </row>
+    <row r="22" s="3" customFormat="1" spans="1:13">
+      <c r="A22" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2176,7 +2206,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="5" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
@@ -2185,298 +2215,298 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="9" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="13" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="13" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D6" s="12"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>87</v>
-      </c>
       <c r="C7" s="11" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D7" s="12"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="9" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B9" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B12" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B14" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B15" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="1" spans="1:3">
       <c r="A18" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" customFormat="1" spans="1:3">
       <c r="A19" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20" customFormat="1" spans="1:3">
       <c r="A20" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" customFormat="1" spans="1:3">
       <c r="A21" s="13" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" customFormat="1" spans="1:3">
       <c r="A22" s="13" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="C22" s="11" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" customFormat="1" spans="1:3">
       <c r="A23" s="13" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" customFormat="1" spans="1:3">
       <c r="A24" s="13" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="1:3">
       <c r="A25" s="13" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="1:3">
       <c r="A26" s="13" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" customFormat="1" spans="1:3">
       <c r="A27" s="13" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="1:3">
@@ -2485,57 +2515,57 @@
     </row>
     <row r="29" customFormat="1" spans="1:3">
       <c r="A29" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B29" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="30" customFormat="1" spans="1:3">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:3">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="32" customFormat="1" spans="1:3">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" customFormat="1" spans="1:3">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="3:3">
@@ -2543,380 +2573,380 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B35" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D35" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B36" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" t="s">
         <v>120</v>
-      </c>
-      <c r="B36" t="s">
-        <v>122</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D36" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" t="s">
         <v>120</v>
-      </c>
-      <c r="B37" t="s">
-        <v>123</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D38" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="D39" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="D40" t="s">
         <v>120</v>
-      </c>
-      <c r="B40" t="s">
-        <v>126</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="D40" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
+        <v>124</v>
+      </c>
+      <c r="B41" t="s">
+        <v>131</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" t="s">
         <v>120</v>
-      </c>
-      <c r="B41" t="s">
-        <v>127</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D41" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B42" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D42" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B44" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D44" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B45" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D45" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B46" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B47" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D47" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" t="s">
+        <v>124</v>
+      </c>
+      <c r="B48" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D48" t="s">
         <v>120</v>
-      </c>
-      <c r="B48" t="s">
-        <v>134</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="D48" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
+        <v>124</v>
+      </c>
+      <c r="B49" t="s">
+        <v>139</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" t="s">
         <v>120</v>
-      </c>
-      <c r="B49" t="s">
-        <v>135</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
+        <v>124</v>
+      </c>
+      <c r="B50" t="s">
+        <v>140</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" t="s">
         <v>120</v>
-      </c>
-      <c r="B50" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D50" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="D51" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B52" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="D52" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D53" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D54" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B55" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="D55" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B56" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="D56" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="D57" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B58" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D58" t="s">
         <v>119</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D58" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" t="s">
+        <v>123</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D59" t="s">
         <v>120</v>
-      </c>
-      <c r="B59" t="s">
-        <v>119</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D59" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D60" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D61" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -2935,39 +2965,39 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="44.1111111111111" customWidth="1"/>
-    <col min="2" max="2" width="45.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="51.8888888888889" customWidth="1"/>
     <col min="3" max="3" width="15.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="C2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2998,19 +3028,19 @@
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3018,16 +3048,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -3035,16 +3065,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C3" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F3" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -3052,16 +3082,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F4" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -3069,16 +3099,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3086,13 +3116,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3100,13 +3130,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3114,13 +3144,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3128,13 +3158,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C9" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D9" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3142,13 +3172,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D10" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3156,13 +3186,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D11" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3170,13 +3200,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D12" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3184,13 +3214,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3198,13 +3228,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3212,13 +3242,13 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -3226,13 +3256,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -3240,13 +3270,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -3254,13 +3284,13 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -3268,13 +3298,13 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -3282,13 +3312,13 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D20" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -3296,13 +3326,13 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D21" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -3310,13 +3340,13 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D22" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -3324,13 +3354,13 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C23" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D23" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -3338,18 +3368,18 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C24" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D24" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="4:4">
       <c r="D25" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gn: update bsa forms
</commit_message>
<xml_diff>
--- a/ONCHO/Breeding Site Survey/Ghana/2022 semptember/gn_oncho_bsa_1_vector_community_question_202210.xlsx
+++ b/ONCHO/Breeding Site Survey/Ghana/2022 semptember/gn_oncho_bsa_1_vector_community_question_202210.xlsx
@@ -64,7 +64,7 @@
     <t>c_recorder_id</t>
   </si>
   <si>
-    <t>Enter recorder ID   </t>
+    <t>1. Enter recorder ID   </t>
   </si>
   <si>
     <t>Enter 2-digit recorder code provided to each recorder (person doing the data entry)   </t>
@@ -85,7 +85,7 @@
     <t>c_district</t>
   </si>
   <si>
-    <t>Select district   </t>
+    <t>2. Select district   </t>
   </si>
   <si>
     <t>Select the appropriate district   </t>
@@ -109,7 +109,7 @@
     <t>c_site</t>
   </si>
   <si>
-    <t>Select community name</t>
+    <t>3. Select community name</t>
   </si>
   <si>
     <t>if(selected(${c_district}, 'Other'), false(),true())</t>
@@ -133,7 +133,7 @@
     <t>c_consent</t>
   </si>
   <si>
-    <t>Does this person consent to take part in the study?   </t>
+    <t>4. Does this person consent to take part in the study?   </t>
   </si>
   <si>
     <t>select_one sex</t>
@@ -142,7 +142,7 @@
     <t>c_gender</t>
   </si>
   <si>
-    <t>What gender is this person?   </t>
+    <t>5. What gender is this person?   </t>
   </si>
   <si>
     <t>${c_consent} = 'Yes'</t>
@@ -151,7 +151,7 @@
     <t>c_age</t>
   </si>
   <si>
-    <t>What age is this person?   </t>
+    <t>6. What age is this person?   </t>
   </si>
   <si>
     <t>. &gt; 0 and . &lt;=120</t>
@@ -163,13 +163,13 @@
     <t>c_occupation</t>
   </si>
   <si>
-    <t>What is their occupation?   </t>
+    <t>7. What is their occupation?   </t>
   </si>
   <si>
     <t>c_how_lng_lived</t>
   </si>
   <si>
-    <t>How long has this person lived in this community?   </t>
+    <t>8. How long has this person lived in this community?   </t>
   </si>
   <si>
     <t>. &lt;= ${c_age}</t>
@@ -184,7 +184,7 @@
     <t>c_black_fly_problem</t>
   </si>
   <si>
-    <t>Are black fly bites a problem in the community? </t>
+    <t>9. Are black fly bites a problem in the community? </t>
   </si>
   <si>
     <t>select_one bite_number</t>
@@ -193,7 +193,7 @@
     <t>c_bites_number</t>
   </si>
   <si>
-    <t>Bites number    </t>
+    <t>10. Bites number    </t>
   </si>
   <si>
     <t>If yes, how many bites do you receive each day?</t>
@@ -202,13 +202,13 @@
     <t>${c_consent} = 'Yes' and ${c_black_fly_problem} = 'Yes'</t>
   </si>
   <si>
-    <t>select_one month</t>
+    <t>select_multiple month</t>
   </si>
   <si>
     <t>c_month</t>
   </si>
   <si>
-    <t>Black fly month   </t>
+    <t>11. Black fly month   </t>
   </si>
   <si>
     <t>Select the month or months when the respondent reports blackfly biting is most frequent</t>
@@ -220,19 +220,19 @@
     <t>c_time</t>
   </si>
   <si>
-    <t>Black fly time of day  </t>
+    <t>12. Black fly time of day  </t>
   </si>
   <si>
     <t>c_know_oncho</t>
   </si>
   <si>
-    <t>Onchocerciasis – do you know what onchocerciasis/river blindness is? </t>
+    <t>13. Onchocerciasis – do you know what onchocerciasis/river blindness is? </t>
   </si>
   <si>
     <t>c_oncho_explanation</t>
   </si>
   <si>
-    <t>Can you explain what onchocerciasis/river blindness is? </t>
+    <t>14. Can you explain what onchocerciasis/river blindness is? </t>
   </si>
   <si>
     <t>${c_consent} = 'Yes' and selected(${c_know_oncho}, 'Yes')</t>
@@ -244,7 +244,7 @@
     <t>c_gps</t>
   </si>
   <si>
-    <t>Enter GPS  </t>
+    <t>15. Enter GPS  </t>
   </si>
   <si>
     <t>Collect GPS coordinates - Must be outside to get accurate reading  </t>
@@ -475,10 +475,10 @@
     <t>allow_choice_duplicates</t>
   </si>
   <si>
-    <t>(2022 October) - 1. vector community questionnaire V2</t>
-  </si>
-  <si>
-    <t>gn_oncho_bsa_1_vector_community_question_202210_v2</t>
+    <t>(2022 October) - 1. vector community questionnaire V3</t>
+  </si>
+  <si>
+    <t>gn_oncho_bsa_1_vector_community_question_202210_v3</t>
   </si>
   <si>
     <t>English</t>
@@ -508,9 +508,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -560,9 +560,33 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -574,31 +598,30 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -620,17 +643,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -644,14 +673,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -660,21 +681,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -685,13 +692,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -710,7 +710,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,43 +830,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -770,13 +872,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,103 +890,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -947,21 +947,25 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -977,16 +981,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1006,32 +1010,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1044,145 +1029,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1594,7 +1594,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C18" sqref="C18:D18"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>

</xml_diff>